<commit_message>
adding new tests and rules
</commit_message>
<xml_diff>
--- a/src/main/resources/net/cloudburo/drools/rules/markup-draft.xlsx
+++ b/src/main/resources/net/cloudburo/drools/rules/markup-draft.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t xml:space="preserve">RuleSet</t>
   </si>
@@ -64,6 +64,9 @@
     <t xml:space="preserve">$journey.getDeptLocation().getCountryCode() in ($param)</t>
   </si>
   <si>
+    <t xml:space="preserve">$journey.getArrLocation().getCountryCode() in ($param)</t>
+  </si>
+  <si>
     <t xml:space="preserve">markup.setValue($param);</t>
   </si>
   <si>
@@ -83,6 +86,15 @@
   </si>
   <si>
     <t xml:space="preserve">"10"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">second_rule_on_markup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"FR"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"20"</t>
   </si>
 </sst>
 </file>
@@ -213,18 +225,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.91"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.91"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,6 +248,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="31.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -244,6 +258,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="50.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -261,6 +276,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -268,6 +284,7 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -277,6 +294,9 @@
         <v>10</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>11</v>
       </c>
     </row>
@@ -284,6 +304,9 @@
       <c r="B8" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="C8" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
@@ -292,35 +315,54 @@
       <c r="C9" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="D9" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
multithreading a single session in a test
</commit_message>
<xml_diff>
--- a/src/main/resources/net/cloudburo/drools/rules/markup-draft.xlsx
+++ b/src/main/resources/net/cloudburo/drools/rules/markup-draft.xlsx
@@ -31,13 +31,13 @@
     <t xml:space="preserve">Import</t>
   </si>
   <si>
-    <t xml:space="preserve">net.cloudburo.drools.Journey, net.cloudburo.drools.Location, net.cloudburo.drools.Markup, net.cloudburo.drools.MarkupType</t>
+    <t xml:space="preserve">net.cloudburo.drools.model2.*</t>
   </si>
   <si>
     <t xml:space="preserve">Variables</t>
   </si>
   <si>
-    <t xml:space="preserve">net.cloudburo.drools.Markup markup</t>
+    <t xml:space="preserve">net.cloudburo.drools.model2.Markup markup</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -109,6 +109,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -130,12 +131,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -143,6 +146,7 @@
       <color rgb="FF008000"/>
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -192,7 +196,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -227,8 +231,8 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>